<commit_message>
Adjustment et progression 12/12/24
</commit_message>
<xml_diff>
--- a/contract/Contract_Progression_2425.xlsx
+++ b/contract/Contract_Progression_2425.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/contract/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CB927B-CEFF-CE4B-8F99-54A71F57CFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28C45CD-9FF1-0D43-BE32-B1F3AA35E44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{8D3FF7CB-512B-BE4C-AEB1-BE6E777E249A}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Water Point Committee / Commite Point d'Eau (CPE) console is build for the OREPA and local authorities</t>
   </si>
   <si>
-    <t>user guides is completed, not validated yet</t>
-  </si>
-  <si>
     <t>Data quality check for the consoles and the new structure of the HANWASH portal is validated</t>
   </si>
   <si>
@@ -79,29 +76,6 @@
   </si>
   <si>
     <t>Training session (Haiti Liaison [Marlene, Wildaine, Nixon]; Steering Committee [Barb Spangler]; M&amp;E committee [Tristam]; Ambassador[Fritz, Wildaine]; D7020)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12 accounts from 43</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> need to be created to complete this task</t>
-    </r>
   </si>
   <si>
     <r>
@@ -134,6 +108,32 @@
       </rPr>
       <t>first_name.last_name</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 accounts from 48</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> need to be created to complete this task</t>
+    </r>
+  </si>
+  <si>
+    <t>user guides is completed</t>
   </si>
 </sst>
 </file>
@@ -289,6 +289,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -296,33 +323,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287ECF86-A753-C447-B82E-9EED8E9D1C69}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:F5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,13 +658,13 @@
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
@@ -676,13 +676,13 @@
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
+      <c r="B2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="13">
         <v>1</v>
       </c>
@@ -692,13 +692,13 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
+      <c r="B3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="13">
         <v>1</v>
       </c>
@@ -708,13 +708,13 @@
       <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
+      <c r="B4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
       <c r="G4" s="13">
         <v>1</v>
       </c>
@@ -724,31 +724,31 @@
       <c r="A5" s="8">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+      <c r="B5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="6">
-        <v>0.73</v>
+        <v>0.96</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="B6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="6">
         <v>1</v>
       </c>
@@ -758,33 +758,33 @@
       <c r="A7" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
+      <c r="B7" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="6">
         <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>3</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
+      <c r="B8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="5"/>
     </row>
@@ -792,13 +792,13 @@
       <c r="A9" s="9">
         <v>3</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="4">
         <v>1</v>
       </c>
@@ -808,33 +808,33 @@
       <c r="A10" s="9">
         <v>3</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="4">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="H11" s="5"/>
     </row>

</xml_diff>

<commit_message>
need to close the year
</commit_message>
<xml_diff>
--- a/contract/Contract_Progression_2425.xlsx
+++ b/contract/Contract_Progression_2425.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/contract/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27EEF56-48C2-9441-BE32-3D57216A08F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980ABE29-55A5-4047-B17A-A7870CE638E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{8D3FF7CB-512B-BE4C-AEB1-BE6E777E249A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Deliverables</t>
   </si>
@@ -110,30 +110,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2 accounts from 48</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> need to be created to complete this task</t>
-    </r>
-  </si>
-  <si>
-    <t>user guides is completed</t>
+    <t>Ongoing task</t>
+  </si>
+  <si>
+    <t>Elements were shared and invitation were shared. We will continue with to relaunch to process for the rest of the non responsive members</t>
+  </si>
+  <si>
+    <t>Guides completed and shared</t>
   </si>
 </sst>
 </file>
@@ -253,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -324,6 +307,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,7 +628,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,11 +718,9 @@
       <c r="E5" s="25"/>
       <c r="F5" s="26"/>
       <c r="G5" s="6">
-        <v>0.96</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
@@ -784,9 +768,11 @@
       <c r="E8" s="16"/>
       <c r="F8" s="17"/>
       <c r="G8" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="H8" s="5"/>
+        <v>0.99</v>
+      </c>
+      <c r="H8" s="27" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
@@ -816,13 +802,13 @@
       <c r="E10" s="16"/>
       <c r="F10" s="17"/>
       <c r="G10" s="4">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>3</v>
       </c>
@@ -834,9 +820,11 @@
       <c r="E11" s="16"/>
       <c r="F11" s="17"/>
       <c r="G11" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="H11" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="28" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>

</xml_diff>